<commit_message>
Add combinational parameter testing script and spreadsheet for food conversation
</commit_message>
<xml_diff>
--- a/Extensive/Coffee.xlsx
+++ b/Extensive/Coffee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12100" yWindow="20" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -650,7 +650,7 @@
   <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>